<commit_message>
refactor: restructured bio class and separated getTransactions into multiple functions, rewritten logs.js to fit new function calls
</commit_message>
<xml_diff>
--- a/osea.xlsx
+++ b/osea.xlsx
@@ -397,13 +397,751 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>deviceUserId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>userName</v>
+      </c>
+      <c r="C1" t="str">
+        <v>timeStamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1008</v>
+      </c>
+      <c r="B2" t="str">
+        <v>CESS</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Tue Oct 08 2024 07:56:08 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1008</v>
+      </c>
+      <c r="B3" t="str">
+        <v>CESS</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Tue Oct 08 2024 11:10:06 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1008</v>
+      </c>
+      <c r="B4" t="str">
+        <v>CESS</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Wed Oct 09 2024 08:01:30 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1008</v>
+      </c>
+      <c r="B5" t="str">
+        <v>CESS</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Wed Oct 09 2024 14:17:03 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1008</v>
+      </c>
+      <c r="B6" t="str">
+        <v>CESS</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Thu Oct 10 2024 07:58:08 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B7" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Mon Oct 07 2024 07:53:45 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B8" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Mon Oct 07 2024 17:08:51 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B9" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Tue Oct 08 2024 09:42:02 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B10" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Tue Oct 08 2024 20:59:03 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B11" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Wed Oct 09 2024 07:42:23 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B12" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Wed Oct 09 2024 17:42:25 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>1009</v>
+      </c>
+      <c r="B13" t="str">
+        <v>JOHN</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Thu Oct 10 2024 07:31:53 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B14" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Mon Oct 07 2024 09:06:52 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B15" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Mon Oct 07 2024 18:02:30 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B16" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Tue Oct 08 2024 10:37:32 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B17" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Tue Oct 08 2024 18:00:59 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B18" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Wed Oct 09 2024 08:47:19 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B19" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Wed Oct 09 2024 18:03:59 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>1011</v>
+      </c>
+      <c r="B20" t="str">
+        <v>DEL</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Thu Oct 10 2024 08:50:15 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B21" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Mon Oct 07 2024 09:01:12 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B22" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Mon Oct 07 2024 18:14:31 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B23" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Tue Oct 08 2024 08:50:27 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B24" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Tue Oct 08 2024 18:08:03 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B25" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Wed Oct 09 2024 09:12:02 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B26" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Wed Oct 09 2024 17:41:13 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>5001</v>
+      </c>
+      <c r="B27" t="str">
+        <v>CRISTINE</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Thu Oct 10 2024 08:38:38 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B28" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Mon Oct 07 2024 08:29:58 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B29" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Mon Oct 07 2024 17:06:58 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B30" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Tue Oct 08 2024 07:20:12 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B31" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Tue Oct 08 2024 17:07:02 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B32" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Wed Oct 09 2024 07:01:09 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B33" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Wed Oct 09 2024 18:04:31 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>5004</v>
+      </c>
+      <c r="B34" t="str">
+        <v>RODEL</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Thu Oct 10 2024 07:32:06 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B35" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Mon Oct 07 2024 07:25:50 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B36" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Mon Oct 07 2024 17:01:41 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B37" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Tue Oct 08 2024 07:59:23 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B38" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Tue Oct 08 2024 17:02:47 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B39" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Wed Oct 09 2024 07:34:28 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B40" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Wed Oct 09 2024 17:01:49 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>5008</v>
+      </c>
+      <c r="B41" t="str">
+        <v>MILES</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Thu Oct 10 2024 07:58:14 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B42" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Mon Oct 07 2024 07:08:37 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B43" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Mon Oct 07 2024 17:00:52 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B44" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Tue Oct 08 2024 06:45:42 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B45" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Tue Oct 08 2024 17:00:14 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B46" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Wed Oct 09 2024 06:57:26 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B47" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Wed Oct 09 2024 17:06:56 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>5010</v>
+      </c>
+      <c r="B48" t="str">
+        <v>CORTEJO</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Thu Oct 10 2024 06:49:09 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B49" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Mon Oct 07 2024 07:07:18 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B50" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Mon Oct 07 2024 17:01:06 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B51" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Tue Oct 08 2024 07:00:38 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B52" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Tue Oct 08 2024 17:03:13 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B53" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Wed Oct 09 2024 12:18:31 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B54" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Wed Oct 09 2024 17:06:59 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>5011</v>
+      </c>
+      <c r="B55" t="str">
+        <v>VINCENT</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Thu Oct 10 2024 06:43:39 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B56" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Mon Oct 07 2024 07:02:09 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B57" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Mon Oct 07 2024 17:00:48 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B58" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Tue Oct 08 2024 06:50:41 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B59" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Tue Oct 08 2024 17:00:04 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B60" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Wed Oct 09 2024 06:42:58 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B61" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Wed Oct 09 2024 17:07:07 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>5012</v>
+      </c>
+      <c r="B62" t="str">
+        <v>HARRY</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Thu Oct 10 2024 06:58:23 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>5013</v>
+      </c>
+      <c r="B63" t="str">
+        <v>IRA</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Tue Oct 08 2024 08:46:36 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>5013</v>
+      </c>
+      <c r="B64" t="str">
+        <v>IRA</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Tue Oct 08 2024 17:04:59 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>5013</v>
+      </c>
+      <c r="B65" t="str">
+        <v>IRA</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Wed Oct 09 2024 07:28:46 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>5013</v>
+      </c>
+      <c r="B66" t="str">
+        <v>IRA</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Wed Oct 09 2024 17:03:31 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>5013</v>
+      </c>
+      <c r="B67" t="str">
+        <v>IRA</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Thu Oct 10 2024 07:41:35 GMT+0800 (Philippine Standard Time)</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C67"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>